<commit_message>
Publish the 2021 F1040
</commit_message>
<xml_diff>
--- a/Federal/f1040-2021.xlsx
+++ b/Federal/f1040-2021.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>2019 Form 1040</t>
   </si>
@@ -201,9 +201,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Earned income credit (EIC)</t>
   </si>
   <si>
@@ -228,15 +225,9 @@
     <t>31</t>
   </si>
   <si>
-    <t>Schedule 3, line 13</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
-    <t>Add lines 27 through 31. These are your total other payments and refundable credits</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -322,6 +313,27 @@
   </si>
   <si>
     <t>2020 Estimated tax payments and amount applied from 2020 return</t>
+  </si>
+  <si>
+    <t>27a</t>
+  </si>
+  <si>
+    <t>27b</t>
+  </si>
+  <si>
+    <t>27c</t>
+  </si>
+  <si>
+    <t>Prior year (2019) earned income</t>
+  </si>
+  <si>
+    <t>Nontaxable combat pay election</t>
+  </si>
+  <si>
+    <t>Schedule 3, line 15</t>
+  </si>
+  <si>
+    <t>Add lines 27a and 28 through 31. These are your total other payments and refundable credits</t>
   </si>
 </sst>
 </file>
@@ -1352,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:D42"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1560,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -1579,7 +1591,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="30"/>
@@ -1607,7 +1619,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
@@ -1617,7 +1629,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -1627,7 +1639,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -1637,43 +1649,43 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F23" s="18">
         <f>SUM(F21:F22)</f>
@@ -1699,7 +1711,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -1791,7 +1803,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
@@ -1805,7 +1817,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
@@ -1853,7 +1865,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
@@ -1943,7 +1955,7 @@
         <v>59</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
@@ -1954,41 +1966,41 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="12"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="12"/>
       <c r="F44" s="13"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="12"/>
@@ -1996,13 +2008,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="12"/>
@@ -2010,13 +2022,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="12"/>
@@ -2024,139 +2036,167 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="18">
-        <f>SUM(D43:D47)</f>
-        <v>0</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="13"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F49" s="18">
-        <f>F41+F42+F48</f>
+        <v>67</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="19"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" s="18">
+        <f>D43+SUM(D46:D49)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
       <c r="E51" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F51" s="18">
-        <f>MAX(F49-F37, 0)</f>
+        <f>F41+F42+F50</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52" s="18">
-        <f>F51</f>
-        <v>0</v>
-      </c>
+      <c r="A52" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D53" s="19">
-        <f>F51-F52</f>
+        <v>72</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="18">
+        <f>MAX(F51-F37, 0)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="12"/>
-      <c r="F53" s="13"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="13"/>
+      <c r="A54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" s="18">
+        <f>F53</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="19">
+        <f>F53-F54</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="18">
+        <f>MAX(F37-F51,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F55" s="18">
-        <f>MAX(F37-F49,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="15"/>
+      <c r="C58" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -2189,14 +2229,14 @@
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="B57:D57"/>
     <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2021 F1040 Schedule 1
</commit_message>
<xml_diff>
--- a/Federal/f1040-2021.xlsx
+++ b/Federal/f1040-2021.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
-    <t>2019 Form 1040</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Add lines 27a and 28 through 31. These are your total other payments and refundable credits</t>
+  </si>
+  <si>
+    <t>2021 Form 1040</t>
   </si>
 </sst>
 </file>
@@ -1028,20 +1028,20 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1380,36 +1380,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="12"/>
@@ -1417,27 +1417,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="12"/>
@@ -1445,27 +1445,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>10</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="12"/>
@@ -1473,27 +1473,27 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>14</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="12"/>
@@ -1501,27 +1501,27 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="12"/>
@@ -1529,57 +1529,57 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
       <c r="E14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>25</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="18">
         <f>SUM(F2:F14)</f>
@@ -1588,29 +1588,29 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31">
+      <c r="D16" s="22"/>
+      <c r="E16" s="23">
         <v>10</v>
       </c>
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="18">
         <f>F15-F16</f>
@@ -1618,8 +1618,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>84</v>
+      <c r="A18" s="27" t="s">
+        <v>83</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
@@ -1628,8 +1628,8 @@
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>85</v>
+      <c r="A19" s="27" t="s">
+        <v>84</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -1638,8 +1638,8 @@
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>86</v>
+      <c r="A20" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -1649,43 +1649,43 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F23" s="18">
         <f>SUM(F21:F22)</f>
@@ -1694,29 +1694,29 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>29</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>30</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="18">
         <f>F23+F24</f>
@@ -1725,15 +1725,15 @@
     </row>
     <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="20">
         <f>MAX(F17-F25,0)</f>
@@ -1742,56 +1742,56 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>39</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>40</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>41</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="18">
         <f>F29+F30</f>
@@ -1800,43 +1800,43 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>44</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>45</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F34" s="18">
         <f>F32+F33</f>
@@ -1845,15 +1845,15 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>46</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>47</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F35" s="18">
         <f>F31-F34</f>
@@ -1862,29 +1862,29 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" s="18">
         <f>F35+F36</f>
@@ -1893,13 +1893,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="12"/>
@@ -1907,13 +1907,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C39" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="12"/>
@@ -1921,13 +1921,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="12"/>
@@ -1935,15 +1935,15 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>58</v>
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="24"/>
       <c r="E41" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F41" s="18">
         <f>SUM(D38:D40)</f>
@@ -1952,27 +1952,27 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
       <c r="E42" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="12"/>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="12"/>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="12"/>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="C46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="12"/>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="12"/>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="12"/>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="12"/>
@@ -2064,15 +2064,15 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="24"/>
       <c r="E50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F50" s="18">
         <f>D43+SUM(D46:D49)</f>
@@ -2081,15 +2081,15 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>70</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
       <c r="E51" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F51" s="18">
         <f>F41+F42+F50</f>
@@ -2097,26 +2097,26 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="A52" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
       <c r="E52" s="6"/>
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="24" t="s">
         <v>72</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>73</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="24"/>
       <c r="E53" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F53" s="18">
         <f>MAX(F51-F37, 0)</f>
@@ -2125,15 +2125,15 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="24"/>
       <c r="E54" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F54" s="18">
         <f>F53</f>
@@ -2142,13 +2142,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" s="19">
         <f>F53-F54</f>
@@ -2158,26 +2158,26 @@
       <c r="F55" s="13"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="A56" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
       <c r="E56" s="12"/>
       <c r="F56" s="13"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="24" t="s">
         <v>77</v>
-      </c>
-      <c r="B57" s="24" t="s">
-        <v>78</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
       <c r="E57" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F57" s="18">
         <f>MAX(F37-F51,0)</f>
@@ -2186,13 +2186,13 @@
     </row>
     <row r="58" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="C58" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="14"/>
@@ -2200,23 +2200,14 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="A28:D28"/>
@@ -2229,14 +2220,23 @@
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>